<commit_message>
finilized the models, but the coefficients look weird
</commit_message>
<xml_diff>
--- a/MSDS 411/Unit 01 Moneyball Baseball Problem/Data/DataDictionary_Baseball.xlsx
+++ b/MSDS 411/Unit 01 Moneyball Baseball Problem/Data/DataDictionary_Baseball.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24426"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="6640" yWindow="2940" windowWidth="14800" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t xml:space="preserve">INDEX    </t>
   </si>
@@ -133,13 +138,55 @@
   </si>
   <si>
     <t>Batters hit by pitch (get a free base)</t>
+  </si>
+  <si>
+    <t>TEAM_Batting_H-(2b+3b+4b)</t>
+  </si>
+  <si>
+    <t>TEAM_batting_HPB + BB</t>
+  </si>
+  <si>
+    <t>1B+2*2B+3*3B+4*4B+walks+HBP+Stolen BASes</t>
+  </si>
+  <si>
+    <t>Team_pitching_BB + 4*Team_pitching_HR + Team_Picthin_H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM_BATTING_HR - TEAM_PITCHING_HR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM_BATTING_BB - TEAM_PITCHING_BB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM_PITCHING_SO - TEAM_BATTING_SO </t>
+  </si>
+  <si>
+    <t>free_bases_num</t>
+  </si>
+  <si>
+    <t>team_batting_1B</t>
+  </si>
+  <si>
+    <t>total_bases</t>
+  </si>
+  <si>
+    <t>total_bases_allowed</t>
+  </si>
+  <si>
+    <t>HR_over_OP</t>
+  </si>
+  <si>
+    <t>walks_over_OP</t>
+  </si>
+  <si>
+    <t>SO_over_OP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +202,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +244,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -192,24 +261,56 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -219,8 +320,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="33">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,20 +655,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -544,7 +679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -555,12 +690,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -571,7 +706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -582,7 +717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -593,7 +728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -604,7 +739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -615,7 +750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -626,7 +761,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -637,7 +772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -648,7 +783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -659,7 +794,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -670,7 +805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -681,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
@@ -692,7 +827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -703,7 +838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
@@ -714,7 +849,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -725,9 +860,77 @@
         <v>31</v>
       </c>
     </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -737,9 +940,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -749,8 +957,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>